<commit_message>
passwaord change and staff master changes
</commit_message>
<xml_diff>
--- a/SMSApplication/bin/Debug/Templates/Student Master Template Import.xlsx
+++ b/SMSApplication/bin/Debug/Templates/Student Master Template Import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>S.No.</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>RF ID Card No.</t>
+  </si>
+  <si>
+    <t>Admission No.</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -415,32 +418,36 @@
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import for staff and student master
</commit_message>
<xml_diff>
--- a/SMSApplication/bin/Debug/Templates/Student Master Template Import.xlsx
+++ b/SMSApplication/bin/Debug/Templates/Student Master Template Import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>S.No.</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Blood Group</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Mobile No.</t>
   </si>
   <si>
@@ -43,6 +40,30 @@
   </si>
   <si>
     <t>Admission No.</t>
+  </si>
+  <si>
+    <t>Parent / Guardian Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Address Line - 1</t>
+  </si>
+  <si>
+    <t>Address Line - 2</t>
+  </si>
+  <si>
+    <t>Address Line - 3</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -404,51 +425,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="14" max="14" width="29" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>